<commit_message>
Amélioration de la doc
</commit_message>
<xml_diff>
--- a/Doc/UseCasesScénarios.xlsx
+++ b/Doc/UseCasesScénarios.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -287,7 +287,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="22">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -570,11 +570,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -678,10 +704,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
@@ -702,17 +746,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -996,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E109" sqref="E109"/>
+    <sheetView tabSelected="1" topLeftCell="A91" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,11 +1050,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1106,11 +1147,11 @@
       <c r="C14" s="15"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="35"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
@@ -1174,7 +1215,7 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="40" t="s">
         <v>44</v>
       </c>
       <c r="B28" s="1"/>
@@ -1183,7 +1224,7 @@
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="38"/>
+      <c r="A29" s="44"/>
       <c r="B29" s="1" t="s">
         <v>46</v>
       </c>
@@ -1192,7 +1233,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="47" t="s">
         <v>47</v>
       </c>
       <c r="B30" s="1"/>
@@ -1201,14 +1242,14 @@
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="42"/>
+      <c r="A31" s="48"/>
       <c r="B31" s="1"/>
       <c r="C31" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="A32" s="40" t="s">
         <v>20</v>
       </c>
       <c r="B32" s="1" t="s">
@@ -1219,7 +1260,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="37"/>
+      <c r="A33" s="43"/>
       <c r="B33" s="1" t="s">
         <v>22</v>
       </c>
@@ -1228,7 +1269,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="37"/>
+      <c r="A34" s="43"/>
       <c r="B34" s="1" t="s">
         <v>23</v>
       </c>
@@ -1237,7 +1278,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="37"/>
+      <c r="A35" s="43"/>
       <c r="B35" s="1" t="s">
         <v>24</v>
       </c>
@@ -1246,7 +1287,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="38"/>
+      <c r="A36" s="44"/>
       <c r="B36" s="1" t="s">
         <v>40</v>
       </c>
@@ -1281,8 +1322,8 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C46" s="26"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="40"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="46"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C47" s="26"/>
@@ -1300,11 +1341,11 @@
       <c r="E49" s="18"/>
     </row>
     <row r="50" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="35" t="s">
+      <c r="A50" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B50" s="35"/>
-      <c r="C50" s="35"/>
+      <c r="B50" s="42"/>
+      <c r="C50" s="42"/>
       <c r="D50" s="20"/>
       <c r="E50" s="21"/>
     </row>
@@ -1407,11 +1448,11 @@
       <c r="E60" s="18"/>
     </row>
     <row r="67" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="35" t="s">
+      <c r="A67" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="35"/>
-      <c r="C67" s="35"/>
+      <c r="B67" s="42"/>
+      <c r="C67" s="42"/>
       <c r="D67" s="33"/>
       <c r="E67" s="21"/>
     </row>
@@ -1497,171 +1538,168 @@
       <c r="A76" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B76" s="1"/>
-      <c r="C76" s="2" t="s">
+      <c r="B76" s="35"/>
+      <c r="C76" s="49" t="s">
         <v>54</v>
       </c>
       <c r="D76" s="21"/>
       <c r="E76" s="21"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A77" s="17"/>
-      <c r="B77" s="1"/>
-      <c r="C77" s="2"/>
+    <row r="77" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="37"/>
+      <c r="B77" s="50"/>
+      <c r="C77" s="39"/>
       <c r="D77" s="21"/>
       <c r="E77" s="21"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A78" s="17"/>
-      <c r="B78" s="1"/>
-      <c r="C78" s="2"/>
+      <c r="A78" s="51"/>
+      <c r="B78" s="26"/>
+      <c r="C78" s="26"/>
       <c r="D78" s="21"/>
       <c r="E78" s="21"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A79" s="17"/>
-      <c r="B79" s="1"/>
-      <c r="C79" s="2"/>
+      <c r="A79" s="51"/>
+      <c r="B79" s="26"/>
+      <c r="C79" s="26"/>
       <c r="D79" s="21"/>
       <c r="E79" s="21"/>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A80" s="17"/>
-      <c r="B80" s="1"/>
-      <c r="C80" s="2"/>
+      <c r="A80" s="51"/>
+      <c r="B80" s="26"/>
+      <c r="C80" s="26"/>
       <c r="D80" s="21"/>
       <c r="E80" s="21"/>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A81" s="7"/>
-      <c r="B81" s="1"/>
-      <c r="C81" s="2"/>
+      <c r="A81" s="26"/>
+      <c r="B81" s="26"/>
+      <c r="C81" s="26"/>
       <c r="D81" s="21"/>
       <c r="E81" s="21"/>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A82" s="7"/>
-      <c r="B82" s="1"/>
-      <c r="C82" s="2"/>
+      <c r="A82" s="26"/>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
       <c r="D82" s="21"/>
       <c r="E82" s="21"/>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A83" s="7"/>
-      <c r="B83" s="1"/>
-      <c r="C83" s="2"/>
+      <c r="A83" s="26"/>
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
       <c r="D83" s="21"/>
       <c r="E83" s="21"/>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A84" s="7"/>
-      <c r="B84" s="1"/>
-      <c r="C84" s="2"/>
+      <c r="A84" s="26"/>
+      <c r="B84" s="26"/>
+      <c r="C84" s="26"/>
       <c r="D84" s="21"/>
       <c r="E84" s="21"/>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A85" s="7"/>
-      <c r="B85" s="1"/>
-      <c r="C85" s="2"/>
+      <c r="A85" s="26"/>
+      <c r="B85" s="26"/>
+      <c r="C85" s="26"/>
       <c r="D85" s="21"/>
       <c r="E85" s="21"/>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A86" s="7"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="2"/>
+      <c r="A86" s="26"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="26"/>
       <c r="D86" s="21"/>
       <c r="E86" s="21"/>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A87" s="7"/>
-      <c r="B87" s="1"/>
-      <c r="C87" s="2"/>
+      <c r="A87" s="26"/>
+      <c r="B87" s="26"/>
+      <c r="C87" s="26"/>
       <c r="D87" s="21"/>
       <c r="E87" s="21"/>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A88" s="7"/>
-      <c r="B88" s="1"/>
-      <c r="C88" s="2"/>
+      <c r="A88" s="26"/>
+      <c r="B88" s="26"/>
+      <c r="C88" s="26"/>
       <c r="D88" s="21"/>
       <c r="E88" s="21"/>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A89" s="7"/>
-      <c r="B89" s="1"/>
-      <c r="C89" s="2"/>
+      <c r="A89" s="26"/>
+      <c r="B89" s="26"/>
+      <c r="C89" s="26"/>
       <c r="D89" s="21"/>
       <c r="E89" s="21"/>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A90" s="7"/>
-      <c r="B90" s="1"/>
-      <c r="C90" s="2"/>
+      <c r="A90" s="26"/>
+      <c r="B90" s="26"/>
+      <c r="C90" s="26"/>
       <c r="D90" s="21"/>
       <c r="E90" s="21"/>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A91" s="7"/>
-      <c r="B91" s="1"/>
-      <c r="C91" s="2"/>
+      <c r="A91" s="26"/>
+      <c r="B91" s="26"/>
+      <c r="C91" s="26"/>
       <c r="D91" s="21"/>
       <c r="E91" s="21"/>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A92" s="7"/>
-      <c r="B92" s="1"/>
-      <c r="C92" s="2"/>
+      <c r="A92" s="26"/>
+      <c r="B92" s="26"/>
+      <c r="C92" s="26"/>
       <c r="D92" s="21"/>
       <c r="E92" s="21"/>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A93" s="7"/>
-      <c r="B93" s="1"/>
-      <c r="C93" s="2"/>
+      <c r="A93" s="26"/>
+      <c r="B93" s="26"/>
+      <c r="C93" s="26"/>
       <c r="D93" s="21"/>
       <c r="E93" s="21"/>
     </row>
     <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A94" s="7"/>
-      <c r="B94" s="1"/>
-      <c r="C94" s="2"/>
+      <c r="A94" s="26"/>
+      <c r="B94" s="26"/>
+      <c r="C94" s="26"/>
       <c r="D94" s="21"/>
       <c r="E94" s="21"/>
     </row>
     <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="7"/>
-      <c r="B95" s="1"/>
-      <c r="C95" s="2"/>
+      <c r="A95" s="26"/>
+      <c r="B95" s="26"/>
+      <c r="C95" s="26"/>
       <c r="D95" s="21"/>
       <c r="E95" s="21"/>
     </row>
     <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="7"/>
-      <c r="B96" s="1"/>
-      <c r="C96" s="2"/>
+      <c r="A96" s="26"/>
+      <c r="B96" s="26"/>
+      <c r="C96" s="26"/>
       <c r="D96" s="21"/>
       <c r="E96" s="21"/>
     </row>
     <row r="97" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="7"/>
-      <c r="B97" s="1"/>
-      <c r="C97" s="2"/>
+      <c r="A97" s="26"/>
+      <c r="B97" s="26"/>
+      <c r="C97" s="26"/>
       <c r="D97" s="21"/>
       <c r="E97" s="21"/>
     </row>
     <row r="98" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="7"/>
-      <c r="B98" s="1"/>
-      <c r="C98" s="2"/>
+      <c r="A98" s="26"/>
+      <c r="B98" s="26"/>
+      <c r="C98" s="26"/>
       <c r="D98" s="21"/>
       <c r="E98" s="21"/>
     </row>
-    <row r="99" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="8"/>
-      <c r="B99" s="13"/>
-      <c r="C99" s="15"/>
+    <row r="99" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D99" s="21"/>
       <c r="E99" s="21"/>
     </row>
@@ -1686,11 +1724,11 @@
       <c r="E103" s="24"/>
     </row>
     <row r="104" spans="1:5" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A104" s="35" t="s">
+      <c r="A104" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="B104" s="35"/>
-      <c r="C104" s="35"/>
+      <c r="B104" s="42"/>
+      <c r="C104" s="42"/>
       <c r="D104" s="22"/>
       <c r="E104" s="24"/>
     </row>
@@ -1761,17 +1799,17 @@
       <c r="B111" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C111" s="43" t="s">
+      <c r="C111" s="36" t="s">
         <v>7</v>
       </c>
       <c r="D111" s="22"/>
       <c r="E111" s="24"/>
     </row>
     <row r="112" spans="1:5" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A112" s="36" t="s">
+      <c r="A112" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="B112" s="45"/>
+      <c r="B112" s="38"/>
       <c r="C112" s="1" t="s">
         <v>56</v>
       </c>
@@ -1779,9 +1817,9 @@
       <c r="E112" s="24"/>
     </row>
     <row r="113" spans="1:5" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="44"/>
+      <c r="A113" s="41"/>
       <c r="B113" s="13"/>
-      <c r="C113" s="46" t="s">
+      <c r="C113" s="39" t="s">
         <v>36</v>
       </c>
       <c r="D113" s="22"/>
@@ -1951,16 +1989,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="A50:C50"/>
+    <mergeCell ref="A67:C67"/>
+    <mergeCell ref="A28:A29"/>
+    <mergeCell ref="A30:A31"/>
     <mergeCell ref="A112:A113"/>
     <mergeCell ref="A104:C104"/>
     <mergeCell ref="A32:A36"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A19:C19"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="A50:C50"/>
-    <mergeCell ref="A67:C67"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A30:A31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="152" orientation="portrait" r:id="rId1"/>

</xml_diff>